<commit_message>
Updated project files for Brainwave Matrix Task 1
</commit_message>
<xml_diff>
--- a/techzone_sales_data.xlsx
+++ b/techzone_sales_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mk199\OneDrive\Desktop\Ronak\Internship\Brainwave Matrix Solutions\Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9A2A56-E03D-4F59-8B71-DF748C56F66A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846D5326-4084-4AA8-8B42-CE11ABC05620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{B155DE68-28A8-4FA1-8B51-8BFB80454E25}"/>
   </bookViews>
@@ -1154,7 +1154,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'TechZone Sales Dashboard'!$AB$3</c:f>
+              <c:f>'TechZone Sales Dashboard'!$AG$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1238,7 +1238,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'TechZone Sales Dashboard'!$AA$4:$AA$7</c:f>
+              <c:f>'TechZone Sales Dashboard'!$AF$4:$AF$7</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1255,7 +1255,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'TechZone Sales Dashboard'!$AB$4:$AB$7</c:f>
+              <c:f>'TechZone Sales Dashboard'!$AG$4:$AG$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1716,7 +1716,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'TechZone Sales Dashboard'!$AB$10</c:f>
+              <c:f>'TechZone Sales Dashboard'!$AG$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1912,7 +1912,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'TechZone Sales Dashboard'!$AA$11:$AA$15</c:f>
+              <c:f>'TechZone Sales Dashboard'!$AF$11:$AF$15</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1932,7 +1932,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'TechZone Sales Dashboard'!$AB$11:$AB$15</c:f>
+              <c:f>'TechZone Sales Dashboard'!$AG$11:$AG$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2373,7 +2373,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'TechZone Sales Dashboard'!$AB$17</c:f>
+              <c:f>'TechZone Sales Dashboard'!$AG$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2587,7 +2587,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'TechZone Sales Dashboard'!$AA$18:$AA$24</c:f>
+              <c:f>'TechZone Sales Dashboard'!$AF$18:$AF$24</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -2613,7 +2613,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'TechZone Sales Dashboard'!$AB$18:$AB$24</c:f>
+              <c:f>'TechZone Sales Dashboard'!$AG$18:$AG$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -3486,7 +3486,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'TechZone Sales Dashboard'!$AB$26</c:f>
+              <c:f>'TechZone Sales Dashboard'!$AG$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3947,7 +3947,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'TechZone Sales Dashboard'!$AA$27:$AA$36</c:f>
+              <c:f>'TechZone Sales Dashboard'!$AF$27:$AF$36</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -3982,7 +3982,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'TechZone Sales Dashboard'!$AB$27:$AB$36</c:f>
+              <c:f>'TechZone Sales Dashboard'!$AG$27:$AG$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -6468,13 +6468,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>409222</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
@@ -6504,13 +6504,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>957438</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>22577</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>155222</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>169333</xdr:rowOff>
@@ -6540,13 +6540,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>486833</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>77611</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>156634</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>105833</xdr:rowOff>
@@ -6576,13 +6576,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>390525</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>911225</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
@@ -6612,13 +6612,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>374649</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>146050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>169332</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
@@ -6685,18 +6685,18 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>42333</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>402167</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="$AD$4">
+    <xdr:sp macro="" textlink="$AI$4">
       <xdr:nvSpPr>
         <xdr:cNvPr id="7" name="Rectangle: Rounded Corners 6">
           <a:extLst>
@@ -6777,18 +6777,18 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>488244</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>35279</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>155222</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>172862</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="$AD$7">
+    <xdr:sp macro="" textlink="$AI$7">
       <xdr:nvSpPr>
         <xdr:cNvPr id="8" name="Rectangle: Rounded Corners 7">
           <a:extLst>
@@ -6869,13 +6869,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>230717</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>85372</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>225778</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>119945</xdr:rowOff>
@@ -6947,13 +6947,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>220133</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>166511</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>28222</xdr:rowOff>
@@ -7025,13 +7025,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>218015</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>136172</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>239889</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>134056</xdr:rowOff>
@@ -8382,7 +8382,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BC7FB201-2C49-433D-845D-48DF8B542176}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
-  <location ref="AA26:AB36" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <location ref="AF26:AG36" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField numFmtId="14" showAll="0"/>
     <pivotField showAll="0"/>
@@ -8573,7 +8573,7 @@
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{47A694D5-122C-4B27-8532-431F9BDF111E}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
-  <location ref="AA17:AB24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <location ref="AF17:AG24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField numFmtId="14" showAll="0"/>
     <pivotField showAll="0"/>
@@ -8705,7 +8705,7 @@
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2F22EEC7-7090-4430-A6B7-3C1F65435771}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
-  <location ref="AA10:AB15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <location ref="AF10:AG15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField numFmtId="14" showAll="0"/>
     <pivotField showAll="0"/>
@@ -8845,7 +8845,7 @@
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FEC6E51B-F8CC-4C31-9505-C32D2B62C224}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="13">
-  <location ref="AA3:AB7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <location ref="AF3:AG7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField numFmtId="14" showAll="0"/>
     <pivotField showAll="0"/>
@@ -9324,273 +9324,273 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79608B8C-E275-4ACC-9AA4-88569D7BC9A5}">
-  <dimension ref="AA3:AD36"/>
+  <dimension ref="AF3:AI36"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="X12" sqref="X12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.90625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="27:30" x14ac:dyDescent="0.35">
-      <c r="AA3" s="2" t="s">
+    <row r="3" spans="32:35" x14ac:dyDescent="0.35">
+      <c r="AF3" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AG3" t="s">
         <v>138</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AI3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="27:30" x14ac:dyDescent="0.35">
-      <c r="AA4" s="3" t="s">
+    <row r="4" spans="32:35" x14ac:dyDescent="0.35">
+      <c r="AF4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="AB4" s="4">
+      <c r="AG4" s="4">
         <v>131200</v>
       </c>
-      <c r="AD4">
+      <c r="AI4">
         <v>11821200</v>
       </c>
     </row>
-    <row r="5" spans="27:30" x14ac:dyDescent="0.35">
-      <c r="AA5" s="3" t="s">
+    <row r="5" spans="32:35" x14ac:dyDescent="0.35">
+      <c r="AF5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AB5" s="4">
+      <c r="AG5" s="4">
         <v>4770000</v>
       </c>
     </row>
-    <row r="6" spans="27:30" x14ac:dyDescent="0.35">
-      <c r="AA6" s="3" t="s">
+    <row r="6" spans="32:35" x14ac:dyDescent="0.35">
+      <c r="AF6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AB6" s="4">
+      <c r="AG6" s="4">
         <v>6920000</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AI6" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="27:30" x14ac:dyDescent="0.35">
-      <c r="AA7" s="3" t="s">
+    <row r="7" spans="32:35" x14ac:dyDescent="0.35">
+      <c r="AF7" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="AB7" s="4">
+      <c r="AG7" s="4">
         <v>11821200</v>
       </c>
-      <c r="AD7">
+      <c r="AI7">
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="27:30" x14ac:dyDescent="0.35">
-      <c r="AA10" s="2" t="s">
+    <row r="10" spans="32:35" x14ac:dyDescent="0.35">
+      <c r="AF10" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AG10" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="27:30" x14ac:dyDescent="0.35">
-      <c r="AA11" s="3" t="s">
+    <row r="11" spans="32:35" x14ac:dyDescent="0.35">
+      <c r="AF11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AB11" s="4">
+      <c r="AG11" s="4">
         <v>3337000</v>
       </c>
     </row>
-    <row r="12" spans="27:30" x14ac:dyDescent="0.35">
-      <c r="AA12" s="3" t="s">
+    <row r="12" spans="32:35" x14ac:dyDescent="0.35">
+      <c r="AF12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AB12" s="4">
+      <c r="AG12" s="4">
         <v>2735200</v>
       </c>
     </row>
-    <row r="13" spans="27:30" x14ac:dyDescent="0.35">
-      <c r="AA13" s="3" t="s">
+    <row r="13" spans="32:35" x14ac:dyDescent="0.35">
+      <c r="AF13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AB13" s="4">
+      <c r="AG13" s="4">
         <v>3965900</v>
       </c>
     </row>
-    <row r="14" spans="27:30" x14ac:dyDescent="0.35">
-      <c r="AA14" s="3" t="s">
+    <row r="14" spans="32:35" x14ac:dyDescent="0.35">
+      <c r="AF14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AB14" s="4">
+      <c r="AG14" s="4">
         <v>1783100</v>
       </c>
     </row>
-    <row r="15" spans="27:30" x14ac:dyDescent="0.35">
-      <c r="AA15" s="3" t="s">
+    <row r="15" spans="32:35" x14ac:dyDescent="0.35">
+      <c r="AF15" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="AB15" s="4">
+      <c r="AG15" s="4">
         <v>11821200</v>
       </c>
     </row>
-    <row r="17" spans="27:28" x14ac:dyDescent="0.35">
-      <c r="AA17" s="2" t="s">
+    <row r="17" spans="32:33" x14ac:dyDescent="0.35">
+      <c r="AF17" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="AB17" t="s">
+      <c r="AG17" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="27:28" x14ac:dyDescent="0.35">
-      <c r="AA18" s="3" t="s">
+    <row r="18" spans="32:33" x14ac:dyDescent="0.35">
+      <c r="AF18" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="AB18" s="4">
+      <c r="AG18" s="4">
         <v>1290100</v>
       </c>
     </row>
-    <row r="19" spans="27:28" x14ac:dyDescent="0.35">
-      <c r="AA19" s="3" t="s">
+    <row r="19" spans="32:33" x14ac:dyDescent="0.35">
+      <c r="AF19" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="AB19" s="4">
+      <c r="AG19" s="4">
         <v>3438300</v>
       </c>
     </row>
-    <row r="20" spans="27:28" x14ac:dyDescent="0.35">
-      <c r="AA20" s="3" t="s">
+    <row r="20" spans="32:33" x14ac:dyDescent="0.35">
+      <c r="AF20" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="AB20" s="4">
+      <c r="AG20" s="4">
         <v>1948700</v>
       </c>
     </row>
-    <row r="21" spans="27:28" x14ac:dyDescent="0.35">
-      <c r="AA21" s="3" t="s">
+    <row r="21" spans="32:33" x14ac:dyDescent="0.35">
+      <c r="AF21" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="AB21" s="4">
+      <c r="AG21" s="4">
         <v>1756700</v>
       </c>
     </row>
-    <row r="22" spans="27:28" x14ac:dyDescent="0.35">
-      <c r="AA22" s="3" t="s">
+    <row r="22" spans="32:33" x14ac:dyDescent="0.35">
+      <c r="AF22" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="AB22" s="4">
+      <c r="AG22" s="4">
         <v>1245100</v>
       </c>
     </row>
-    <row r="23" spans="27:28" x14ac:dyDescent="0.35">
-      <c r="AA23" s="3" t="s">
+    <row r="23" spans="32:33" x14ac:dyDescent="0.35">
+      <c r="AF23" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="AB23" s="4">
+      <c r="AG23" s="4">
         <v>2142300</v>
       </c>
     </row>
-    <row r="24" spans="27:28" x14ac:dyDescent="0.35">
-      <c r="AA24" s="3" t="s">
+    <row r="24" spans="32:33" x14ac:dyDescent="0.35">
+      <c r="AF24" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="AB24" s="4">
+      <c r="AG24" s="4">
         <v>11821200</v>
       </c>
     </row>
-    <row r="26" spans="27:28" x14ac:dyDescent="0.35">
-      <c r="AA26" s="2" t="s">
+    <row r="26" spans="32:33" x14ac:dyDescent="0.35">
+      <c r="AF26" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="AB26" t="s">
+      <c r="AG26" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="27" spans="27:28" x14ac:dyDescent="0.35">
-      <c r="AA27" s="3" t="s">
+    <row r="27" spans="32:33" x14ac:dyDescent="0.35">
+      <c r="AF27" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AB27" s="4">
+      <c r="AG27" s="4">
         <v>48900</v>
       </c>
     </row>
-    <row r="28" spans="27:28" x14ac:dyDescent="0.35">
-      <c r="AA28" s="3" t="s">
+    <row r="28" spans="32:33" x14ac:dyDescent="0.35">
+      <c r="AF28" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AB28" s="4">
+      <c r="AG28" s="4">
         <v>1410000</v>
       </c>
     </row>
-    <row r="29" spans="27:28" x14ac:dyDescent="0.35">
-      <c r="AA29" s="3" t="s">
+    <row r="29" spans="32:33" x14ac:dyDescent="0.35">
+      <c r="AF29" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AB29" s="4">
+      <c r="AG29" s="4">
         <v>1590000</v>
       </c>
     </row>
-    <row r="30" spans="27:28" x14ac:dyDescent="0.35">
-      <c r="AA30" s="3" t="s">
+    <row r="30" spans="32:33" x14ac:dyDescent="0.35">
+      <c r="AF30" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AB30" s="4">
+      <c r="AG30" s="4">
         <v>2340000</v>
       </c>
     </row>
-    <row r="31" spans="27:28" x14ac:dyDescent="0.35">
-      <c r="AA31" s="3" t="s">
+    <row r="31" spans="32:33" x14ac:dyDescent="0.35">
+      <c r="AF31" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AB31" s="4">
+      <c r="AG31" s="4">
         <v>53100</v>
       </c>
     </row>
-    <row r="32" spans="27:28" x14ac:dyDescent="0.35">
-      <c r="AA32" s="3" t="s">
+    <row r="32" spans="32:33" x14ac:dyDescent="0.35">
+      <c r="AF32" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AB32" s="4">
+      <c r="AG32" s="4">
         <v>1770000</v>
       </c>
     </row>
-    <row r="33" spans="27:28" x14ac:dyDescent="0.35">
-      <c r="AA33" s="3" t="s">
+    <row r="33" spans="32:33" x14ac:dyDescent="0.35">
+      <c r="AF33" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AB33" s="4">
+      <c r="AG33" s="4">
         <v>2695000</v>
       </c>
     </row>
-    <row r="34" spans="27:28" x14ac:dyDescent="0.35">
-      <c r="AA34" s="3" t="s">
+    <row r="34" spans="32:33" x14ac:dyDescent="0.35">
+      <c r="AF34" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AB34" s="4">
+      <c r="AG34" s="4">
         <v>1885000</v>
       </c>
     </row>
-    <row r="35" spans="27:28" x14ac:dyDescent="0.35">
-      <c r="AA35" s="3" t="s">
+    <row r="35" spans="32:33" x14ac:dyDescent="0.35">
+      <c r="AF35" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AB35" s="4">
+      <c r="AG35" s="4">
         <v>29200</v>
       </c>
     </row>
-    <row r="36" spans="27:28" x14ac:dyDescent="0.35">
-      <c r="AA36" s="3" t="s">
+    <row r="36" spans="32:33" x14ac:dyDescent="0.35">
+      <c r="AF36" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="AB36" s="4">
+      <c r="AG36" s="4">
         <v>11821200</v>
       </c>
     </row>

</xml_diff>